<commit_message>
added velocity graph and commentary
</commit_message>
<xml_diff>
--- a/Release 2 Docs/BurndownChart 2.xlsx
+++ b/Release 2 Docs/BurndownChart 2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James Tuerlings\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James Tuerlings\repos\Group_IFB299\Release 2 Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>Date</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>talk about extra points</t>
+  </si>
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>Velocity</t>
   </si>
 </sst>
 </file>
@@ -140,7 +146,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -148,14 +154,15 @@
     <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -449,11 +456,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1006097408"/>
-        <c:axId val="1006097952"/>
+        <c:axId val="1258272992"/>
+        <c:axId val="1258267008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1006097408"/>
+        <c:axId val="1258272992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -566,12 +573,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1006097952"/>
+        <c:crossAx val="1258267008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1006097952"/>
+        <c:axId val="1258267008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -684,7 +691,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1006097408"/>
+        <c:crossAx val="1258272992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1104,11 +1111,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1006094688"/>
-        <c:axId val="1006095232"/>
+        <c:axId val="1258276256"/>
+        <c:axId val="1258270816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1006094688"/>
+        <c:axId val="1258276256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1221,12 +1228,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1006095232"/>
+        <c:crossAx val="1258270816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1006095232"/>
+        <c:axId val="1258270816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1339,7 +1346,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1006094688"/>
+        <c:crossAx val="1258276256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1824,11 +1831,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1100987712"/>
-        <c:axId val="1100989888"/>
+        <c:axId val="1258268640"/>
+        <c:axId val="1258269728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1100987712"/>
+        <c:axId val="1258268640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1941,12 +1948,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1100989888"/>
+        <c:crossAx val="1258269728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1100989888"/>
+        <c:axId val="1258269728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2064,7 +2071,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1100987712"/>
+        <c:crossAx val="1258268640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2593,11 +2600,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1211101760"/>
-        <c:axId val="1211093600"/>
+        <c:axId val="1258275168"/>
+        <c:axId val="1258277344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1211101760"/>
+        <c:axId val="1258275168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2717,12 +2724,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1211093600"/>
+        <c:crossAx val="1258277344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1211093600"/>
+        <c:axId val="1258277344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2842,7 +2849,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1211101760"/>
+        <c:crossAx val="1258275168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2895,6 +2902,651 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Velocity for</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> each Sprint - Group 114</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Velocity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{C7C79BC2-7411-4AE1-A5BD-37B8A6E4EFFE}" type="YVALUE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[Y VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-AU"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{5979B999-5EC0-43DE-8C64-2F6039C05DEA}" type="YVALUE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[Y VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-AU"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{680847EE-BCAC-4B51-B349-11674733B359}" type="YVALUE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[Y VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-AU"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{7D3E5472-89C4-45CC-899F-69EAAE38F408}" type="YVALUE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[Y VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-AU"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="r"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1314076176"/>
+        <c:axId val="1314072912"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1314076176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Sprint</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1314072912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1314072912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Story Points Completed</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1314076176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="2"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -3092,6 +3744,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4641,6 +5333,522 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5250,16 +6458,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1299883</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>145677</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>224118</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>22412</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>123265</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>168089</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5273,6 +6481,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1639150</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>42658</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>177363</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>35935</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5639,10 +6877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A19:S38"/>
+  <dimension ref="A1:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19:S38"/>
+    <sheetView tabSelected="1" topLeftCell="I62" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5656,6 +6894,46 @@
     <col min="17" max="17" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>14</v>
+      </c>
+    </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="Q19" s="4" t="s">
         <v>0</v>
@@ -5668,11 +6946,11 @@
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
@@ -5682,7 +6960,7 @@
       <c r="I20" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="L20" s="9">
+      <c r="L20" s="7">
         <v>42606</v>
       </c>
       <c r="M20">
@@ -5691,7 +6969,7 @@
       <c r="N20">
         <v>25</v>
       </c>
-      <c r="Q20" s="9">
+      <c r="Q20" s="7">
         <v>42606</v>
       </c>
       <c r="R20">
@@ -5722,7 +7000,7 @@
       <c r="I21" s="2">
         <v>24</v>
       </c>
-      <c r="L21" s="10">
+      <c r="L21" s="8">
         <v>42613</v>
       </c>
       <c r="M21">
@@ -5731,7 +7009,7 @@
       <c r="N21">
         <v>18</v>
       </c>
-      <c r="Q21" s="10">
+      <c r="Q21" s="8">
         <v>42613</v>
       </c>
       <c r="R21">
@@ -5762,7 +7040,7 @@
       <c r="I22" s="2">
         <v>23</v>
       </c>
-      <c r="L22" s="10">
+      <c r="L22" s="8">
         <v>42620</v>
       </c>
       <c r="M22">
@@ -5771,7 +7049,7 @@
       <c r="N22">
         <v>12</v>
       </c>
-      <c r="Q22" s="10">
+      <c r="Q22" s="8">
         <v>42620</v>
       </c>
       <c r="R22">
@@ -5802,7 +7080,7 @@
       <c r="I23" s="2">
         <v>17</v>
       </c>
-      <c r="L23" s="10">
+      <c r="L23" s="8">
         <v>42627</v>
       </c>
       <c r="M23">
@@ -5811,7 +7089,7 @@
       <c r="N23">
         <v>6</v>
       </c>
-      <c r="Q23" s="10">
+      <c r="Q23" s="8">
         <v>42627</v>
       </c>
       <c r="R23">
@@ -5842,7 +7120,7 @@
       <c r="I24" s="2">
         <v>12</v>
       </c>
-      <c r="L24" s="10">
+      <c r="L24" s="8">
         <v>42634</v>
       </c>
       <c r="M24">
@@ -5920,11 +7198,11 @@
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
       <c r="G27" s="5">
         <v>42658</v>
       </c>

</xml_diff>